<commit_message>
update vai2 task dem
</commit_message>
<xml_diff>
--- a/Document/TaskSheet.xlsx
+++ b/Document/TaskSheet.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="13395" windowHeight="3735"/>
+    <workbookView xWindow="360" yWindow="420" windowWidth="13395" windowHeight="3615"/>
   </bookViews>
   <sheets>
     <sheet name="150525-150526" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="44">
   <si>
     <t>No.</t>
   </si>
@@ -99,17 +99,82 @@
     <t>fix database, class, usecase</t>
   </si>
   <si>
-    <t>head/footer user</t>
-  </si>
-  <si>
-    <t>login page</t>
+    <t>fix database v2</t>
+  </si>
+  <si>
+    <t>html adminPage</t>
+  </si>
+  <si>
+    <t>html accountDetailPage</t>
+  </si>
+  <si>
+    <t>html header/footer user</t>
+  </si>
+  <si>
+    <t>DatNC, TrieuLH,Anh,Toan</t>
+  </si>
+  <si>
+    <t>TrieuLH,DatNC</t>
+  </si>
+  <si>
+    <t>interface dashboard Manager</t>
+  </si>
+  <si>
+    <t>interface dashboard Staff</t>
+  </si>
+  <si>
+    <t>html directorPage</t>
+  </si>
+  <si>
+    <t>html projectDetailPage</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CODE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="128"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> login page</t>
+    </r>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>create flow Page</t>
+  </si>
+  <si>
+    <t>admin header/footer html</t>
+  </si>
+  <si>
+    <t>Không có css</t>
+  </si>
+  <si>
+    <t>bỏ page này gộp chung với adminpage</t>
+  </si>
+  <si>
+    <t>tách skill với category hoặc gộp lại.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -134,8 +199,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -157,6 +244,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -201,7 +300,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -232,6 +331,25 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -533,18 +651,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N24"/>
+  <dimension ref="A1:N170"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="I28" sqref="I28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="15" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="21.42578125" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" customWidth="1"/>
+    <col min="11" max="11" width="11.85546875" style="17" customWidth="1"/>
     <col min="13" max="13" width="6.140625" customWidth="1"/>
     <col min="14" max="14" width="18.42578125" customWidth="1"/>
   </cols>
@@ -580,6 +699,9 @@
       <c r="J1" s="4" t="s">
         <v>16</v>
       </c>
+      <c r="K1" s="16" t="s">
+        <v>38</v>
+      </c>
       <c r="M1" s="1"/>
       <c r="N1" s="1" t="s">
         <v>15</v>
@@ -610,6 +732,7 @@
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="4"/>
+      <c r="K2" s="16"/>
       <c r="M2" s="8" t="s">
         <v>0</v>
       </c>
@@ -642,6 +765,7 @@
       </c>
       <c r="I3" s="6"/>
       <c r="J3" s="4"/>
+      <c r="K3" s="16"/>
       <c r="M3" s="6">
         <v>1</v>
       </c>
@@ -672,6 +796,7 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="4"/>
+      <c r="K4" s="16"/>
       <c r="M4" s="6">
         <v>2</v>
       </c>
@@ -702,6 +827,7 @@
       </c>
       <c r="I5" s="6"/>
       <c r="J5" s="4"/>
+      <c r="K5" s="16"/>
       <c r="M5" s="6">
         <v>3</v>
       </c>
@@ -728,6 +854,7 @@
       <c r="J6" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="K6" s="16"/>
       <c r="M6" s="6">
         <v>4</v>
       </c>
@@ -754,12 +881,13 @@
       <c r="J7" s="4" t="s">
         <v>18</v>
       </c>
+      <c r="K7" s="16"/>
       <c r="M7" s="6">
         <v>5</v>
       </c>
       <c r="N7" s="6"/>
     </row>
-    <row r="8" spans="1:14">
+    <row r="8" spans="1:14" ht="75">
       <c r="A8" s="5">
         <v>7</v>
       </c>
@@ -773,10 +901,11 @@
       <c r="G8" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H8" s="6"/>
+      <c r="H8" s="10"/>
       <c r="I8" s="6"/>
-      <c r="J8" s="4" t="s">
-        <v>18</v>
+      <c r="J8" s="4"/>
+      <c r="K8" s="16" t="s">
+        <v>43</v>
       </c>
       <c r="M8" s="6">
         <v>6</v>
@@ -794,12 +923,17 @@
       <c r="D9" s="6"/>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
-      <c r="G9" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="6"/>
+      <c r="G9" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="10">
+        <v>42151</v>
+      </c>
       <c r="I9" s="6"/>
-      <c r="J9" s="4"/>
+      <c r="J9" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K9" s="16"/>
       <c r="M9" s="6">
         <v>7</v>
       </c>
@@ -815,13 +949,18 @@
       </c>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="10">
+        <v>42151</v>
+      </c>
       <c r="I10" s="6"/>
-      <c r="J10" s="4"/>
+      <c r="J10" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K10" s="16"/>
       <c r="M10" s="6">
         <v>8</v>
       </c>
@@ -837,15 +976,18 @@
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
-      <c r="F11" s="11" t="s">
+      <c r="F11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
+      <c r="H11" s="10">
+        <v>42151</v>
+      </c>
       <c r="I11" s="6"/>
       <c r="J11" s="4" t="s">
-        <v>18</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="K11" s="16"/>
       <c r="M11" s="6">
         <v>9</v>
       </c>
@@ -861,13 +1003,18 @@
       </c>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
-      <c r="F12" s="11" t="s">
+      <c r="F12" s="13" t="s">
         <v>11</v>
       </c>
       <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
+      <c r="H12" s="10">
+        <v>42151</v>
+      </c>
       <c r="I12" s="6"/>
-      <c r="J12" s="4"/>
+      <c r="J12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K12" s="16"/>
       <c r="M12" s="6">
         <v>10</v>
       </c>
@@ -887,9 +1034,10 @@
       <c r="G13" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="6"/>
+      <c r="H13" s="10"/>
       <c r="I13" s="6"/>
       <c r="J13" s="4"/>
+      <c r="K13" s="16"/>
       <c r="M13" s="6">
         <v>11</v>
       </c>
@@ -903,15 +1051,22 @@
       <c r="C14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="D14" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="E14" s="6"/>
+      <c r="D14" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>11</v>
+      </c>
       <c r="F14" s="6"/>
       <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
+      <c r="H14" s="10">
+        <v>42152</v>
+      </c>
       <c r="I14" s="6"/>
-      <c r="J14" s="4"/>
+      <c r="J14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K14" s="16"/>
       <c r="M14" s="6">
         <v>12</v>
       </c>
@@ -923,17 +1078,22 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="7" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D15" s="6"/>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
+      <c r="H15" s="10">
+        <v>42152</v>
+      </c>
       <c r="I15" s="6"/>
-      <c r="J15" s="4"/>
+      <c r="J15" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K15" s="16"/>
       <c r="M15" s="6">
         <v>13</v>
       </c>
@@ -944,38 +1104,50 @@
         <v>15</v>
       </c>
       <c r="B16" s="6"/>
-      <c r="C16" s="7" t="s">
-        <v>28</v>
+      <c r="C16" s="14" t="s">
+        <v>37</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="13" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
+      <c r="H16" s="10">
+        <v>42152</v>
+      </c>
       <c r="I16" s="6"/>
       <c r="J16" s="4" t="s">
         <v>3</v>
       </c>
+      <c r="K16" s="16"/>
       <c r="M16" s="6">
         <v>14</v>
       </c>
       <c r="N16" s="6"/>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:14" ht="60">
       <c r="A17" s="5">
         <v>16</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
+      <c r="C17" s="7" t="s">
+        <v>29</v>
+      </c>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
+      <c r="F17" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
+      <c r="H17" s="10">
+        <v>42152</v>
+      </c>
       <c r="I17" s="6"/>
       <c r="J17" s="4"/>
+      <c r="K17" s="16" t="s">
+        <v>42</v>
+      </c>
       <c r="M17" s="6">
         <v>15</v>
       </c>
@@ -986,32 +1158,50 @@
         <v>17</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
+      <c r="C18" s="7" t="s">
+        <v>27</v>
+      </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
+      <c r="E18" s="12" t="s">
+        <v>11</v>
+      </c>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
+      <c r="H18" s="10">
+        <v>42152</v>
+      </c>
       <c r="I18" s="6"/>
-      <c r="J18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K18" s="16"/>
       <c r="M18" s="6">
         <v>16</v>
       </c>
       <c r="N18" s="6"/>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:14" ht="30">
       <c r="A19" s="5">
         <v>18</v>
       </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
+      <c r="C19" s="7" t="s">
+        <v>28</v>
+      </c>
       <c r="D19" s="6"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
+      <c r="H19" s="10">
+        <v>42152</v>
+      </c>
       <c r="I19" s="6"/>
       <c r="J19" s="4"/>
+      <c r="K19" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="M19" s="6">
         <v>17</v>
       </c>
@@ -1022,14 +1212,21 @@
         <v>19</v>
       </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
+      <c r="C20" s="7" t="s">
+        <v>33</v>
+      </c>
       <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
+      <c r="E20" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
+      <c r="H20" s="10">
+        <v>42152</v>
+      </c>
       <c r="I20" s="6"/>
       <c r="J20" s="4"/>
+      <c r="K20" s="16"/>
       <c r="M20" s="6">
         <v>18</v>
       </c>
@@ -1040,14 +1237,21 @@
         <v>20</v>
       </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
+      <c r="C21" s="7" t="s">
+        <v>34</v>
+      </c>
       <c r="D21" s="6"/>
-      <c r="E21" s="6"/>
+      <c r="E21" s="11" t="s">
+        <v>11</v>
+      </c>
       <c r="F21" s="6"/>
       <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
+      <c r="H21" s="10">
+        <v>42152</v>
+      </c>
       <c r="I21" s="6"/>
       <c r="J21" s="4"/>
+      <c r="K21" s="16"/>
       <c r="M21" s="6">
         <v>19</v>
       </c>
@@ -1058,14 +1262,19 @@
         <v>21</v>
       </c>
       <c r="B22" s="6"/>
-      <c r="C22" s="7"/>
+      <c r="C22" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="D22" s="6"/>
       <c r="E22" s="6"/>
       <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
+      <c r="G22" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="10"/>
       <c r="I22" s="6"/>
       <c r="J22" s="4"/>
+      <c r="K22" s="16"/>
       <c r="M22" s="6">
         <v>20</v>
       </c>
@@ -1076,22 +1285,1440 @@
         <v>22</v>
       </c>
       <c r="B23" s="6"/>
-      <c r="C23" s="7"/>
+      <c r="C23" s="7" t="s">
+        <v>36</v>
+      </c>
       <c r="D23" s="6"/>
       <c r="E23" s="6"/>
       <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
+      <c r="G23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="10"/>
       <c r="I23" s="6"/>
       <c r="J23" s="4"/>
+      <c r="K23" s="16"/>
       <c r="M23" s="6">
         <v>21</v>
       </c>
       <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14">
+      <c r="A24" s="5">
+        <v>23</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="10">
+        <v>42152</v>
+      </c>
+      <c r="I24" s="6"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="16"/>
       <c r="M24" s="2"/>
       <c r="N24" s="2"/>
+    </row>
+    <row r="25" spans="1:14">
+      <c r="A25" s="5">
+        <v>24</v>
+      </c>
+      <c r="B25" s="6"/>
+      <c r="C25" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
+      <c r="G25" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H25" s="10">
+        <v>42152</v>
+      </c>
+      <c r="I25" s="6"/>
+      <c r="J25" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K25" s="16"/>
+    </row>
+    <row r="26" spans="1:14">
+      <c r="A26" s="5">
+        <v>25</v>
+      </c>
+      <c r="B26" s="6"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="6"/>
+      <c r="I26" s="6"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="16"/>
+    </row>
+    <row r="27" spans="1:14">
+      <c r="A27" s="5">
+        <v>26</v>
+      </c>
+      <c r="B27" s="6"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
+      <c r="H27" s="6"/>
+      <c r="I27" s="6"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="16"/>
+    </row>
+    <row r="28" spans="1:14">
+      <c r="A28" s="5">
+        <v>27</v>
+      </c>
+      <c r="B28" s="6"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="6"/>
+      <c r="I28" s="6"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="16"/>
+    </row>
+    <row r="29" spans="1:14">
+      <c r="A29" s="5">
+        <v>28</v>
+      </c>
+      <c r="B29" s="6"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="16"/>
+    </row>
+    <row r="30" spans="1:14">
+      <c r="A30" s="5">
+        <v>29</v>
+      </c>
+      <c r="B30" s="6"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="16"/>
+    </row>
+    <row r="31" spans="1:14">
+      <c r="A31" s="5">
+        <v>30</v>
+      </c>
+      <c r="B31" s="6"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+      <c r="J31" s="4"/>
+      <c r="K31" s="16"/>
+    </row>
+    <row r="32" spans="1:14">
+      <c r="A32" s="5">
+        <v>31</v>
+      </c>
+      <c r="B32" s="6"/>
+      <c r="C32" s="7"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="6"/>
+      <c r="I32" s="6"/>
+      <c r="J32" s="4"/>
+      <c r="K32" s="16"/>
+    </row>
+    <row r="33" spans="1:11">
+      <c r="A33" s="5">
+        <v>32</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="6"/>
+      <c r="I33" s="6"/>
+      <c r="J33" s="4"/>
+      <c r="K33" s="16"/>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" s="5">
+        <v>33</v>
+      </c>
+      <c r="B34" s="6"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+      <c r="F34" s="6"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="16"/>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" s="5">
+        <v>34</v>
+      </c>
+      <c r="B35" s="6"/>
+      <c r="C35" s="7"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="6"/>
+      <c r="I35" s="6"/>
+      <c r="J35" s="4"/>
+      <c r="K35" s="16"/>
+    </row>
+    <row r="36" spans="1:11">
+      <c r="A36" s="5">
+        <v>35</v>
+      </c>
+      <c r="B36" s="6"/>
+      <c r="C36" s="7"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="4"/>
+      <c r="K36" s="16"/>
+    </row>
+    <row r="37" spans="1:11">
+      <c r="A37" s="5">
+        <v>36</v>
+      </c>
+      <c r="B37" s="6"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+      <c r="F37" s="6"/>
+      <c r="G37" s="6"/>
+      <c r="H37" s="6"/>
+      <c r="I37" s="6"/>
+      <c r="J37" s="4"/>
+      <c r="K37" s="16"/>
+    </row>
+    <row r="38" spans="1:11">
+      <c r="A38" s="5">
+        <v>37</v>
+      </c>
+      <c r="B38" s="6"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="6"/>
+      <c r="H38" s="6"/>
+      <c r="I38" s="6"/>
+      <c r="J38" s="4"/>
+      <c r="K38" s="16"/>
+    </row>
+    <row r="39" spans="1:11">
+      <c r="A39" s="5">
+        <v>38</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="6"/>
+      <c r="I39" s="6"/>
+      <c r="J39" s="4"/>
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:11">
+      <c r="A40" s="5">
+        <v>39</v>
+      </c>
+      <c r="B40" s="6"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+      <c r="F40" s="6"/>
+      <c r="G40" s="6"/>
+      <c r="H40" s="6"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="16"/>
+    </row>
+    <row r="41" spans="1:11">
+      <c r="A41" s="5">
+        <v>40</v>
+      </c>
+      <c r="B41" s="6"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+      <c r="F41" s="6"/>
+      <c r="G41" s="6"/>
+      <c r="H41" s="6"/>
+      <c r="I41" s="6"/>
+      <c r="J41" s="4"/>
+      <c r="K41" s="16"/>
+    </row>
+    <row r="42" spans="1:11">
+      <c r="A42" s="5">
+        <v>41</v>
+      </c>
+      <c r="B42" s="6"/>
+      <c r="C42" s="7"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+      <c r="F42" s="6"/>
+      <c r="G42" s="6"/>
+      <c r="H42" s="6"/>
+      <c r="I42" s="6"/>
+      <c r="J42" s="4"/>
+      <c r="K42" s="16"/>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" s="5">
+        <v>42</v>
+      </c>
+      <c r="B43" s="6"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="4"/>
+      <c r="K43" s="16"/>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" s="5">
+        <v>43</v>
+      </c>
+      <c r="B44" s="6"/>
+      <c r="C44" s="7"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="6"/>
+      <c r="I44" s="6"/>
+      <c r="J44" s="4"/>
+      <c r="K44" s="16"/>
+    </row>
+    <row r="45" spans="1:11">
+      <c r="A45" s="5">
+        <v>44</v>
+      </c>
+      <c r="B45" s="6"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="6"/>
+      <c r="I45" s="6"/>
+      <c r="J45" s="4"/>
+      <c r="K45" s="16"/>
+    </row>
+    <row r="46" spans="1:11">
+      <c r="A46" s="5">
+        <v>45</v>
+      </c>
+      <c r="B46" s="6"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+      <c r="F46" s="6"/>
+      <c r="G46" s="6"/>
+      <c r="H46" s="6"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="16"/>
+    </row>
+    <row r="47" spans="1:11">
+      <c r="A47" s="5">
+        <v>46</v>
+      </c>
+      <c r="B47" s="6"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+      <c r="F47" s="6"/>
+      <c r="G47" s="6"/>
+      <c r="H47" s="6"/>
+      <c r="I47" s="6"/>
+      <c r="J47" s="4"/>
+      <c r="K47" s="16"/>
+    </row>
+    <row r="48" spans="1:11">
+      <c r="A48" s="5">
+        <v>47</v>
+      </c>
+      <c r="B48" s="6"/>
+      <c r="C48" s="7"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+      <c r="F48" s="6"/>
+      <c r="G48" s="6"/>
+      <c r="H48" s="6"/>
+      <c r="I48" s="6"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="16"/>
+    </row>
+    <row r="49" spans="1:11">
+      <c r="A49" s="5">
+        <v>48</v>
+      </c>
+      <c r="B49" s="6"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="6"/>
+      <c r="H49" s="6"/>
+      <c r="I49" s="6"/>
+      <c r="J49" s="4"/>
+      <c r="K49" s="16"/>
+    </row>
+    <row r="50" spans="1:11">
+      <c r="A50" s="5">
+        <v>49</v>
+      </c>
+      <c r="B50" s="6"/>
+      <c r="C50" s="7"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="16"/>
+    </row>
+    <row r="51" spans="1:11">
+      <c r="A51" s="5">
+        <v>50</v>
+      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="7"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="4"/>
+      <c r="K51" s="16"/>
+    </row>
+    <row r="52" spans="1:11">
+      <c r="A52" s="5">
+        <v>51</v>
+      </c>
+      <c r="B52" s="6"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+      <c r="F52" s="6"/>
+      <c r="G52" s="6"/>
+      <c r="H52" s="6"/>
+      <c r="I52" s="6"/>
+      <c r="J52" s="4"/>
+      <c r="K52" s="16"/>
+    </row>
+    <row r="53" spans="1:11">
+      <c r="A53" s="5">
+        <v>52</v>
+      </c>
+      <c r="B53" s="6"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="6"/>
+      <c r="E53" s="6"/>
+      <c r="F53" s="6"/>
+      <c r="G53" s="6"/>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
+      <c r="J53" s="4"/>
+      <c r="K53" s="16"/>
+    </row>
+    <row r="54" spans="1:11">
+      <c r="A54" s="5">
+        <v>53</v>
+      </c>
+      <c r="B54" s="6"/>
+      <c r="C54" s="7"/>
+      <c r="D54" s="6"/>
+      <c r="E54" s="6"/>
+      <c r="F54" s="6"/>
+      <c r="G54" s="6"/>
+      <c r="H54" s="6"/>
+      <c r="I54" s="6"/>
+      <c r="J54" s="4"/>
+      <c r="K54" s="16"/>
+    </row>
+    <row r="55" spans="1:11">
+      <c r="A55" s="5">
+        <v>54</v>
+      </c>
+      <c r="B55" s="6"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="6"/>
+      <c r="F55" s="6"/>
+      <c r="G55" s="6"/>
+      <c r="H55" s="6"/>
+      <c r="I55" s="6"/>
+      <c r="J55" s="4"/>
+      <c r="K55" s="16"/>
+    </row>
+    <row r="56" spans="1:11">
+      <c r="A56" s="5">
+        <v>55</v>
+      </c>
+      <c r="B56" s="6"/>
+      <c r="C56" s="7"/>
+      <c r="D56" s="6"/>
+      <c r="E56" s="6"/>
+      <c r="F56" s="6"/>
+      <c r="G56" s="6"/>
+      <c r="H56" s="6"/>
+      <c r="I56" s="6"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="16"/>
+    </row>
+    <row r="57" spans="1:11">
+      <c r="A57" s="5">
+        <v>56</v>
+      </c>
+      <c r="B57" s="6"/>
+      <c r="C57" s="7"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="4"/>
+      <c r="K57" s="16"/>
+    </row>
+    <row r="58" spans="1:11">
+      <c r="A58" s="5">
+        <v>57</v>
+      </c>
+      <c r="B58" s="6"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="6"/>
+      <c r="E58" s="6"/>
+      <c r="F58" s="6"/>
+      <c r="G58" s="6"/>
+      <c r="H58" s="6"/>
+      <c r="I58" s="6"/>
+      <c r="J58" s="4"/>
+      <c r="K58" s="16"/>
+    </row>
+    <row r="59" spans="1:11">
+      <c r="A59" s="5">
+        <v>58</v>
+      </c>
+      <c r="B59" s="6"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="6"/>
+      <c r="E59" s="6"/>
+      <c r="F59" s="6"/>
+      <c r="G59" s="6"/>
+      <c r="H59" s="6"/>
+      <c r="I59" s="6"/>
+      <c r="J59" s="4"/>
+      <c r="K59" s="16"/>
+    </row>
+    <row r="60" spans="1:11">
+      <c r="A60" s="5">
+        <v>59</v>
+      </c>
+      <c r="B60" s="6"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="6"/>
+      <c r="E60" s="6"/>
+      <c r="F60" s="6"/>
+      <c r="G60" s="6"/>
+      <c r="H60" s="6"/>
+      <c r="I60" s="6"/>
+      <c r="J60" s="4"/>
+      <c r="K60" s="16"/>
+    </row>
+    <row r="61" spans="1:11">
+      <c r="A61" s="5">
+        <v>60</v>
+      </c>
+      <c r="B61" s="6"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="6"/>
+      <c r="F61" s="6"/>
+      <c r="G61" s="6"/>
+      <c r="H61" s="6"/>
+      <c r="I61" s="6"/>
+      <c r="J61" s="4"/>
+      <c r="K61" s="16"/>
+    </row>
+    <row r="62" spans="1:11">
+      <c r="A62" s="5">
+        <v>61</v>
+      </c>
+      <c r="B62" s="6"/>
+      <c r="C62" s="7"/>
+      <c r="D62" s="6"/>
+      <c r="E62" s="6"/>
+      <c r="F62" s="6"/>
+      <c r="G62" s="6"/>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="4"/>
+      <c r="K62" s="16"/>
+    </row>
+    <row r="63" spans="1:11">
+      <c r="A63" s="5">
+        <v>62</v>
+      </c>
+      <c r="B63" s="6"/>
+      <c r="C63" s="7"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="6"/>
+      <c r="F63" s="6"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="4"/>
+      <c r="K63" s="16"/>
+    </row>
+    <row r="64" spans="1:11">
+      <c r="A64" s="5">
+        <v>63</v>
+      </c>
+      <c r="B64" s="6"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="4"/>
+      <c r="K64" s="16"/>
+    </row>
+    <row r="65" spans="1:11">
+      <c r="A65" s="5">
+        <v>64</v>
+      </c>
+      <c r="B65" s="6"/>
+      <c r="C65" s="7"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
+      <c r="F65" s="6"/>
+      <c r="G65" s="6"/>
+      <c r="H65" s="6"/>
+      <c r="I65" s="6"/>
+      <c r="J65" s="4"/>
+      <c r="K65" s="16"/>
+    </row>
+    <row r="66" spans="1:11">
+      <c r="A66" s="5">
+        <v>65</v>
+      </c>
+      <c r="B66" s="6"/>
+      <c r="C66" s="7"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
+      <c r="F66" s="6"/>
+      <c r="G66" s="6"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="4"/>
+      <c r="K66" s="16"/>
+    </row>
+    <row r="67" spans="1:11">
+      <c r="A67" s="5">
+        <v>66</v>
+      </c>
+      <c r="B67" s="6"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
+      <c r="F67" s="6"/>
+      <c r="G67" s="6"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="16"/>
+    </row>
+    <row r="68" spans="1:11">
+      <c r="A68" s="5">
+        <v>67</v>
+      </c>
+      <c r="B68" s="6"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="6"/>
+      <c r="E68" s="6"/>
+      <c r="F68" s="6"/>
+      <c r="G68" s="6"/>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="4"/>
+      <c r="K68" s="16"/>
+    </row>
+    <row r="69" spans="1:11">
+      <c r="A69" s="5">
+        <v>68</v>
+      </c>
+      <c r="B69" s="6"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="6"/>
+      <c r="E69" s="6"/>
+      <c r="F69" s="6"/>
+      <c r="G69" s="6"/>
+      <c r="H69" s="6"/>
+      <c r="I69" s="6"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="16"/>
+    </row>
+    <row r="70" spans="1:11">
+      <c r="A70" s="5">
+        <v>69</v>
+      </c>
+      <c r="B70" s="6"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="6"/>
+      <c r="E70" s="6"/>
+      <c r="F70" s="6"/>
+      <c r="G70" s="6"/>
+      <c r="H70" s="6"/>
+      <c r="I70" s="6"/>
+      <c r="J70" s="4"/>
+      <c r="K70" s="16"/>
+    </row>
+    <row r="71" spans="1:11">
+      <c r="A71" s="5">
+        <v>70</v>
+      </c>
+      <c r="B71" s="6"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="4"/>
+      <c r="K71" s="16"/>
+    </row>
+    <row r="72" spans="1:11">
+      <c r="A72" s="5">
+        <v>71</v>
+      </c>
+      <c r="B72" s="6"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="6"/>
+      <c r="E72" s="6"/>
+      <c r="F72" s="6"/>
+      <c r="G72" s="6"/>
+      <c r="H72" s="6"/>
+      <c r="I72" s="6"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="16"/>
+    </row>
+    <row r="73" spans="1:11">
+      <c r="A73" s="5">
+        <v>72</v>
+      </c>
+      <c r="B73" s="6"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="6"/>
+      <c r="E73" s="6"/>
+      <c r="F73" s="6"/>
+      <c r="G73" s="6"/>
+      <c r="H73" s="6"/>
+      <c r="I73" s="6"/>
+      <c r="J73" s="4"/>
+      <c r="K73" s="16"/>
+    </row>
+    <row r="74" spans="1:11">
+      <c r="A74" s="5">
+        <v>73</v>
+      </c>
+      <c r="B74" s="6"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="6"/>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6"/>
+      <c r="G74" s="6"/>
+      <c r="H74" s="6"/>
+      <c r="I74" s="6"/>
+      <c r="J74" s="4"/>
+      <c r="K74" s="16"/>
+    </row>
+    <row r="75" spans="1:11">
+      <c r="A75" s="5">
+        <v>74</v>
+      </c>
+      <c r="B75" s="6"/>
+      <c r="C75" s="7"/>
+      <c r="D75" s="6"/>
+      <c r="E75" s="6"/>
+      <c r="F75" s="6"/>
+      <c r="G75" s="6"/>
+      <c r="H75" s="6"/>
+      <c r="I75" s="6"/>
+      <c r="J75" s="4"/>
+      <c r="K75" s="16"/>
+    </row>
+    <row r="76" spans="1:11">
+      <c r="A76" s="5">
+        <v>75</v>
+      </c>
+      <c r="B76" s="6"/>
+      <c r="C76" s="7"/>
+      <c r="D76" s="6"/>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6"/>
+      <c r="G76" s="6"/>
+      <c r="H76" s="6"/>
+      <c r="I76" s="6"/>
+      <c r="J76" s="4"/>
+      <c r="K76" s="16"/>
+    </row>
+    <row r="77" spans="1:11">
+      <c r="A77" s="5">
+        <v>76</v>
+      </c>
+      <c r="B77" s="6"/>
+      <c r="C77" s="7"/>
+      <c r="D77" s="6"/>
+      <c r="E77" s="6"/>
+      <c r="F77" s="6"/>
+      <c r="G77" s="6"/>
+      <c r="H77" s="6"/>
+      <c r="I77" s="6"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="16"/>
+    </row>
+    <row r="78" spans="1:11">
+      <c r="A78" s="5">
+        <v>77</v>
+      </c>
+      <c r="B78" s="6"/>
+      <c r="C78" s="7"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="4"/>
+      <c r="K78" s="16"/>
+    </row>
+    <row r="79" spans="1:11">
+      <c r="A79" s="5">
+        <v>78</v>
+      </c>
+      <c r="B79" s="6"/>
+      <c r="C79" s="7"/>
+      <c r="D79" s="6"/>
+      <c r="E79" s="6"/>
+      <c r="F79" s="6"/>
+      <c r="G79" s="6"/>
+      <c r="H79" s="6"/>
+      <c r="I79" s="6"/>
+      <c r="J79" s="4"/>
+      <c r="K79" s="16"/>
+    </row>
+    <row r="80" spans="1:11">
+      <c r="A80" s="5">
+        <v>79</v>
+      </c>
+      <c r="B80" s="6"/>
+      <c r="C80" s="7"/>
+      <c r="D80" s="6"/>
+      <c r="E80" s="6"/>
+      <c r="F80" s="6"/>
+      <c r="G80" s="6"/>
+      <c r="H80" s="6"/>
+      <c r="I80" s="6"/>
+      <c r="J80" s="4"/>
+      <c r="K80" s="16"/>
+    </row>
+    <row r="81" spans="1:11">
+      <c r="A81" s="5">
+        <v>80</v>
+      </c>
+      <c r="B81" s="6"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6"/>
+      <c r="G81" s="6"/>
+      <c r="H81" s="6"/>
+      <c r="I81" s="6"/>
+      <c r="J81" s="4"/>
+      <c r="K81" s="16"/>
+    </row>
+    <row r="82" spans="1:11">
+      <c r="A82" s="5">
+        <v>81</v>
+      </c>
+      <c r="B82" s="6"/>
+      <c r="C82" s="7"/>
+      <c r="D82" s="6"/>
+      <c r="E82" s="6"/>
+      <c r="F82" s="6"/>
+      <c r="G82" s="6"/>
+      <c r="H82" s="6"/>
+      <c r="I82" s="6"/>
+      <c r="J82" s="4"/>
+      <c r="K82" s="16"/>
+    </row>
+    <row r="83" spans="1:11">
+      <c r="A83" s="5">
+        <v>82</v>
+      </c>
+      <c r="B83" s="6"/>
+      <c r="C83" s="7"/>
+      <c r="D83" s="6"/>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6"/>
+      <c r="G83" s="6"/>
+      <c r="H83" s="6"/>
+      <c r="I83" s="6"/>
+      <c r="J83" s="4"/>
+      <c r="K83" s="16"/>
+    </row>
+    <row r="84" spans="1:11">
+      <c r="A84" s="5">
+        <v>83</v>
+      </c>
+      <c r="B84" s="6"/>
+      <c r="C84" s="7"/>
+      <c r="D84" s="6"/>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6"/>
+      <c r="G84" s="6"/>
+      <c r="H84" s="6"/>
+      <c r="I84" s="6"/>
+      <c r="J84" s="4"/>
+      <c r="K84" s="16"/>
+    </row>
+    <row r="85" spans="1:11">
+      <c r="A85" s="5">
+        <v>84</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="7"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="4"/>
+      <c r="K85" s="16"/>
+    </row>
+    <row r="86" spans="1:11">
+      <c r="A86" s="5">
+        <v>85</v>
+      </c>
+      <c r="B86" s="6"/>
+      <c r="C86" s="7"/>
+      <c r="D86" s="6"/>
+      <c r="E86" s="6"/>
+      <c r="F86" s="6"/>
+      <c r="G86" s="6"/>
+      <c r="H86" s="6"/>
+      <c r="I86" s="6"/>
+      <c r="J86" s="4"/>
+      <c r="K86" s="16"/>
+    </row>
+    <row r="87" spans="1:11">
+      <c r="A87" s="5">
+        <v>86</v>
+      </c>
+      <c r="B87" s="6"/>
+      <c r="C87" s="7"/>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="6"/>
+      <c r="G87" s="6"/>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="16"/>
+    </row>
+    <row r="88" spans="1:11">
+      <c r="A88" s="5">
+        <v>87</v>
+      </c>
+      <c r="B88" s="6"/>
+      <c r="C88" s="7"/>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="6"/>
+      <c r="G88" s="6"/>
+      <c r="H88" s="6"/>
+      <c r="I88" s="6"/>
+      <c r="J88" s="4"/>
+      <c r="K88" s="16"/>
+    </row>
+    <row r="89" spans="1:11">
+      <c r="A89" s="5">
+        <v>88</v>
+      </c>
+      <c r="B89" s="6"/>
+      <c r="C89" s="7"/>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="6"/>
+      <c r="G89" s="6"/>
+      <c r="H89" s="6"/>
+      <c r="I89" s="6"/>
+      <c r="J89" s="4"/>
+      <c r="K89" s="16"/>
+    </row>
+    <row r="90" spans="1:11">
+      <c r="A90" s="5">
+        <v>89</v>
+      </c>
+      <c r="B90" s="6"/>
+      <c r="C90" s="7"/>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="6"/>
+      <c r="G90" s="6"/>
+      <c r="H90" s="6"/>
+      <c r="I90" s="6"/>
+      <c r="J90" s="4"/>
+      <c r="K90" s="16"/>
+    </row>
+    <row r="91" spans="1:11">
+      <c r="A91" s="5">
+        <v>90</v>
+      </c>
+      <c r="B91" s="6"/>
+      <c r="C91" s="7"/>
+      <c r="D91" s="6"/>
+      <c r="E91" s="6"/>
+      <c r="F91" s="6"/>
+      <c r="G91" s="6"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="16"/>
+    </row>
+    <row r="92" spans="1:11">
+      <c r="A92" s="5">
+        <v>91</v>
+      </c>
+      <c r="B92" s="6"/>
+      <c r="C92" s="7"/>
+      <c r="D92" s="6"/>
+      <c r="E92" s="6"/>
+      <c r="F92" s="6"/>
+      <c r="G92" s="6"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="4"/>
+      <c r="K92" s="16"/>
+    </row>
+    <row r="93" spans="1:11">
+      <c r="A93" s="5">
+        <v>92</v>
+      </c>
+      <c r="B93" s="6"/>
+      <c r="C93" s="7"/>
+      <c r="D93" s="6"/>
+      <c r="E93" s="6"/>
+      <c r="F93" s="6"/>
+      <c r="G93" s="6"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="4"/>
+      <c r="K93" s="16"/>
+    </row>
+    <row r="94" spans="1:11">
+      <c r="A94" s="5">
+        <v>93</v>
+      </c>
+      <c r="B94" s="6"/>
+      <c r="C94" s="7"/>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6"/>
+      <c r="F94" s="6"/>
+      <c r="G94" s="6"/>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="4"/>
+      <c r="K94" s="16"/>
+    </row>
+    <row r="95" spans="1:11">
+      <c r="A95" s="5">
+        <v>94</v>
+      </c>
+      <c r="B95" s="6"/>
+      <c r="C95" s="7"/>
+      <c r="D95" s="6"/>
+      <c r="E95" s="6"/>
+      <c r="F95" s="6"/>
+      <c r="G95" s="6"/>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="4"/>
+      <c r="K95" s="16"/>
+    </row>
+    <row r="96" spans="1:11">
+      <c r="A96" s="5">
+        <v>95</v>
+      </c>
+      <c r="B96" s="6"/>
+      <c r="C96" s="7"/>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6"/>
+      <c r="F96" s="6"/>
+      <c r="G96" s="6"/>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="4"/>
+      <c r="K96" s="16"/>
+    </row>
+    <row r="97" spans="1:11">
+      <c r="A97" s="5">
+        <v>96</v>
+      </c>
+      <c r="B97" s="6"/>
+      <c r="C97" s="7"/>
+      <c r="D97" s="6"/>
+      <c r="E97" s="6"/>
+      <c r="F97" s="6"/>
+      <c r="G97" s="6"/>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="4"/>
+      <c r="K97" s="16"/>
+    </row>
+    <row r="98" spans="1:11">
+      <c r="A98" s="5">
+        <v>97</v>
+      </c>
+      <c r="B98" s="6"/>
+      <c r="C98" s="7"/>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6"/>
+      <c r="F98" s="6"/>
+      <c r="G98" s="6"/>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="16"/>
+    </row>
+    <row r="99" spans="1:11">
+      <c r="A99" s="5">
+        <v>98</v>
+      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="7"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="4"/>
+      <c r="K99" s="16"/>
+    </row>
+    <row r="100" spans="1:11">
+      <c r="A100" s="5">
+        <v>99</v>
+      </c>
+      <c r="B100" s="6"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6"/>
+      <c r="F100" s="6"/>
+      <c r="G100" s="15"/>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="4"/>
+      <c r="K100" s="16"/>
+    </row>
+    <row r="101" spans="1:11">
+      <c r="A101" s="5">
+        <v>100</v>
+      </c>
+      <c r="B101" s="6"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="6"/>
+      <c r="E101" s="6"/>
+      <c r="F101" s="6"/>
+      <c r="G101" s="15"/>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="4"/>
+      <c r="K101" s="16"/>
+    </row>
+    <row r="102" spans="1:11">
+      <c r="A102" s="5">
+        <v>101</v>
+      </c>
+      <c r="B102" s="6"/>
+      <c r="C102" s="7"/>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6"/>
+      <c r="F102" s="6"/>
+      <c r="G102" s="15"/>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="16"/>
+    </row>
+    <row r="103" spans="1:11">
+      <c r="A103" s="5">
+        <v>102</v>
+      </c>
+      <c r="B103" s="6"/>
+      <c r="C103" s="7"/>
+      <c r="D103" s="6"/>
+      <c r="E103" s="6"/>
+      <c r="F103" s="6"/>
+      <c r="G103" s="15"/>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="4"/>
+      <c r="K103" s="16"/>
+    </row>
+    <row r="104" spans="1:11">
+      <c r="G104" s="18"/>
+    </row>
+    <row r="105" spans="1:11">
+      <c r="G105" s="18"/>
+    </row>
+    <row r="106" spans="1:11">
+      <c r="G106" s="18"/>
+    </row>
+    <row r="107" spans="1:11">
+      <c r="G107" s="18"/>
+    </row>
+    <row r="108" spans="1:11">
+      <c r="G108" s="18"/>
+    </row>
+    <row r="109" spans="1:11">
+      <c r="G109" s="18"/>
+    </row>
+    <row r="110" spans="1:11">
+      <c r="G110" s="18"/>
+    </row>
+    <row r="111" spans="1:11">
+      <c r="G111" s="18"/>
+    </row>
+    <row r="112" spans="1:11">
+      <c r="G112" s="18"/>
+    </row>
+    <row r="113" spans="7:7">
+      <c r="G113" s="18"/>
+    </row>
+    <row r="114" spans="7:7">
+      <c r="G114" s="18"/>
+    </row>
+    <row r="115" spans="7:7">
+      <c r="G115" s="18"/>
+    </row>
+    <row r="116" spans="7:7">
+      <c r="G116" s="18"/>
+    </row>
+    <row r="117" spans="7:7">
+      <c r="G117" s="18"/>
+    </row>
+    <row r="118" spans="7:7">
+      <c r="G118" s="18"/>
+    </row>
+    <row r="119" spans="7:7">
+      <c r="G119" s="18"/>
+    </row>
+    <row r="120" spans="7:7">
+      <c r="G120" s="18"/>
+    </row>
+    <row r="121" spans="7:7">
+      <c r="G121" s="18"/>
+    </row>
+    <row r="122" spans="7:7">
+      <c r="G122" s="18"/>
+    </row>
+    <row r="123" spans="7:7">
+      <c r="G123" s="18"/>
+    </row>
+    <row r="124" spans="7:7">
+      <c r="G124" s="18"/>
+    </row>
+    <row r="125" spans="7:7">
+      <c r="G125" s="18"/>
+    </row>
+    <row r="126" spans="7:7">
+      <c r="G126" s="18"/>
+    </row>
+    <row r="127" spans="7:7">
+      <c r="G127" s="18"/>
+    </row>
+    <row r="128" spans="7:7">
+      <c r="G128" s="18"/>
+    </row>
+    <row r="129" spans="7:7">
+      <c r="G129" s="18"/>
+    </row>
+    <row r="130" spans="7:7">
+      <c r="G130" s="18"/>
+    </row>
+    <row r="131" spans="7:7">
+      <c r="G131" s="18"/>
+    </row>
+    <row r="132" spans="7:7">
+      <c r="G132" s="18"/>
+    </row>
+    <row r="133" spans="7:7">
+      <c r="G133" s="18"/>
+    </row>
+    <row r="134" spans="7:7">
+      <c r="G134" s="18"/>
+    </row>
+    <row r="135" spans="7:7">
+      <c r="G135" s="18"/>
+    </row>
+    <row r="136" spans="7:7">
+      <c r="G136" s="18"/>
+    </row>
+    <row r="137" spans="7:7">
+      <c r="G137" s="18"/>
+    </row>
+    <row r="138" spans="7:7">
+      <c r="G138" s="18"/>
+    </row>
+    <row r="139" spans="7:7">
+      <c r="G139" s="18"/>
+    </row>
+    <row r="140" spans="7:7">
+      <c r="G140" s="18"/>
+    </row>
+    <row r="141" spans="7:7">
+      <c r="G141" s="18"/>
+    </row>
+    <row r="142" spans="7:7">
+      <c r="G142" s="18"/>
+    </row>
+    <row r="143" spans="7:7">
+      <c r="G143" s="18"/>
+    </row>
+    <row r="144" spans="7:7">
+      <c r="G144" s="18"/>
+    </row>
+    <row r="145" spans="7:7">
+      <c r="G145" s="18"/>
+    </row>
+    <row r="146" spans="7:7">
+      <c r="G146" s="18"/>
+    </row>
+    <row r="147" spans="7:7">
+      <c r="G147" s="18"/>
+    </row>
+    <row r="148" spans="7:7">
+      <c r="G148" s="18"/>
+    </row>
+    <row r="149" spans="7:7">
+      <c r="G149" s="18"/>
+    </row>
+    <row r="150" spans="7:7">
+      <c r="G150" s="18"/>
+    </row>
+    <row r="151" spans="7:7">
+      <c r="G151" s="18"/>
+    </row>
+    <row r="152" spans="7:7">
+      <c r="G152" s="18"/>
+    </row>
+    <row r="153" spans="7:7">
+      <c r="G153" s="18"/>
+    </row>
+    <row r="154" spans="7:7">
+      <c r="G154" s="18"/>
+    </row>
+    <row r="155" spans="7:7">
+      <c r="G155" s="18"/>
+    </row>
+    <row r="156" spans="7:7">
+      <c r="G156" s="18"/>
+    </row>
+    <row r="157" spans="7:7">
+      <c r="G157" s="18"/>
+    </row>
+    <row r="158" spans="7:7">
+      <c r="G158" s="18"/>
+    </row>
+    <row r="159" spans="7:7">
+      <c r="G159" s="18"/>
+    </row>
+    <row r="160" spans="7:7">
+      <c r="G160" s="18"/>
+    </row>
+    <row r="161" spans="7:7">
+      <c r="G161" s="18"/>
+    </row>
+    <row r="162" spans="7:7">
+      <c r="G162" s="18"/>
+    </row>
+    <row r="163" spans="7:7">
+      <c r="G163" s="18"/>
+    </row>
+    <row r="164" spans="7:7">
+      <c r="G164" s="18"/>
+    </row>
+    <row r="165" spans="7:7">
+      <c r="G165" s="18"/>
+    </row>
+    <row r="166" spans="7:7">
+      <c r="G166" s="18"/>
+    </row>
+    <row r="167" spans="7:7">
+      <c r="G167" s="18"/>
+    </row>
+    <row r="168" spans="7:7">
+      <c r="G168" s="18"/>
+    </row>
+    <row r="169" spans="7:7">
+      <c r="G169" s="18"/>
+    </row>
+    <row r="170" spans="7:7">
+      <c r="G170" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>